<commit_message>
Added tutorial.ipynb and refined the repositroy
</commit_message>
<xml_diff>
--- a/output/goods_shipping_company_alpha_relations_matrix.xlsx
+++ b/output/goods_shipping_company_alpha_relations_matrix.xlsx
@@ -440,27 +440,27 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Evaluate Size of Order (EO)</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Ship Outside of EU (SO)</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>Receive Order(RO)</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Generate Standard Bill (GB)</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Load Container (LC)</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Evaluate Size of Order (EO)</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Ship Outside of EU (SO)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -492,12 +492,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -559,12 +559,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>←</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -596,22 +596,22 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>←</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -628,12 +628,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Receive Order(RO)</t>
+          <t>Evaluate Size of Order (EO)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>→</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -653,12 +653,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>←</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -668,24 +668,24 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Generate Standard Bill (GB)</t>
+          <t>Ship Outside of EU (SO)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -695,12 +695,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -710,29 +710,29 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>||</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>←</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Load Container (LC)</t>
+          <t>Receive Order(RO)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -747,17 +747,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>→</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -777,14 +777,14 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Evaluate Size of Order (EO)</t>
+          <t>Generate Standard Bill (GB)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -794,12 +794,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>→</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -809,12 +809,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>||</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -836,7 +836,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ship Outside of EU (SO)</t>
+          <t>Load Container (LC)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>→</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -856,12 +856,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>→</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>→</t>
         </is>
       </c>
     </row>
@@ -908,17 +908,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>||</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>||</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>←</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>←</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">

</xml_diff>